<commit_message>
Signed-off-by: Krits Huang <47982451+Krstar233@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Front-end/vue-back-ManageSystem/static/data.xlsx
+++ b/Front-end/vue-back-ManageSystem/static/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23028" windowHeight="10020"/>
+    <workbookView windowWidth="23040" windowHeight="9564"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>一级分类</t>
   </si>
@@ -24,34 +24,58 @@
     <t>二级分类</t>
   </si>
   <si>
-    <t>前端开发</t>
-  </si>
-  <si>
-    <t>JavaScript</t>
-  </si>
-  <si>
-    <t>Vue</t>
-  </si>
-  <si>
-    <t>Node.js</t>
-  </si>
-  <si>
-    <t>React</t>
-  </si>
-  <si>
-    <t>后端开发</t>
-  </si>
-  <si>
-    <t>spring MVC</t>
-  </si>
-  <si>
-    <t>mybatis</t>
-  </si>
-  <si>
-    <t>数据库开发</t>
-  </si>
-  <si>
-    <t>mysql</t>
+    <t>教育/语言</t>
+  </si>
+  <si>
+    <t>雅思</t>
+  </si>
+  <si>
+    <t>托福</t>
+  </si>
+  <si>
+    <t>四级</t>
+  </si>
+  <si>
+    <t>六级</t>
+  </si>
+  <si>
+    <t>理学/工学</t>
+  </si>
+  <si>
+    <t>物理</t>
+  </si>
+  <si>
+    <t>化学</t>
+  </si>
+  <si>
+    <t>数学</t>
+  </si>
+  <si>
+    <t>计算机</t>
+  </si>
+  <si>
+    <t>C语言</t>
+  </si>
+  <si>
+    <t>数据结构</t>
+  </si>
+  <si>
+    <t>文学/艺术</t>
+  </si>
+  <si>
+    <t>绘画</t>
+  </si>
+  <si>
+    <t>历史</t>
+  </si>
+  <si>
+    <t>医学</t>
+  </si>
+  <si>
+    <t>骨科</t>
+  </si>
+  <si>
+    <t>人体</t>
   </si>
 </sst>
 </file>
@@ -64,19 +88,12 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -95,13 +112,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -112,14 +122,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -143,6 +145,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -150,12 +159,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -163,31 +195,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -195,30 +234,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,187 +250,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,20 +470,20 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,6 +503,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -496,21 +528,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -529,148 +546,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1026,13 +1043,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1092,10 +1109,58 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>